<commit_message>
Update standard score conversions and remove temp file
Updated the Standard_Score_Conversions.xlsx file with new data and removed a temporary Excel file from Analyses_covered.
</commit_message>
<xml_diff>
--- a/static/Datasets/Standard_Scores/Standard_Score_Conversions.xlsx
+++ b/static/Datasets/Standard_Scores/Standard_Score_Conversions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmyszkowski/Documents/GitHub/personal-website-2022/static/Datasets/Standard_Scores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C34224-E05D-0A4F-8011-9CBFD46C1CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1DD479-BDBF-984E-A42A-F510C33F4EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21560" xr2:uid="{6B7937FC-4FE7-6A44-935C-F99D5EC29F35}"/>
   </bookViews>
@@ -621,12 +621,8 @@
         <f>IF(COUNTBLANK(B2:D2)+COUNTBLANK(C8:D8)=0,B$4*D8+C8,"(fill above and right)")</f>
         <v>(fill above and right)</v>
       </c>
-      <c r="C8" s="3">
-        <v>500</v>
-      </c>
-      <c r="D8" s="3">
-        <v>100</v>
-      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>